<commit_message>
[dev] test 2 and update get_result function
</commit_message>
<xml_diff>
--- a/BestModelsList.xlsx
+++ b/BestModelsList.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Conv</t>
   </si>
@@ -68,16 +68,20 @@
   </si>
   <si>
     <t>128x128</t>
+  </si>
+  <si>
+    <t>256x256</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d.m.yyyy"/>
+    <numFmt numFmtId="165" formatCode="dd.mm.yyyy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -93,6 +97,10 @@
     <font>
       <sz val="18.0"/>
       <color rgb="FF0C0C0C"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -121,7 +129,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border/>
     <border>
       <left/>
@@ -132,16 +140,11 @@
       <top/>
       <bottom/>
     </border>
-    <border>
-      <right/>
-      <top/>
-      <bottom/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -149,7 +152,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
@@ -159,10 +161,12 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -394,7 +398,6 @@
     <col customWidth="1" min="11" max="11" width="13.86"/>
     <col customWidth="1" min="12" max="12" width="13.14"/>
     <col customWidth="1" min="13" max="13" width="13.0"/>
-    <col customWidth="1" min="14" max="26" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -402,97 +405,138 @@
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="2"/>
+      <c r="F1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
-      <c r="I1" s="3"/>
+      <c r="I1" s="2"/>
       <c r="J1" s="1"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
-      <c r="M1" s="3"/>
+      <c r="M1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="7">
+      <c r="A3" s="6">
         <v>45626.0</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="7">
         <v>0.0</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="7">
         <v>0.0</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="7">
         <v>0.0</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="7">
         <v>0.0</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="8">
+      <c r="K3" s="7">
         <v>128.0</v>
       </c>
-      <c r="L3" s="8">
+      <c r="L3" s="7">
         <v>50.0</v>
       </c>
-      <c r="M3" s="8" t="b">
+      <c r="M3" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="8">
+        <v>45597.0</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="9">
+        <v>0.0</v>
+      </c>
+      <c r="G4" s="9">
+        <v>0.0</v>
+      </c>
+      <c r="H4" s="9">
+        <v>0.0</v>
+      </c>
+      <c r="I4" s="9">
+        <v>0.0</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="9">
+        <v>128.0</v>
+      </c>
+      <c r="L4" s="9">
+        <v>50.0</v>
+      </c>
+      <c r="M4" s="9" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>